<commit_message>
Added quality control system suitability
</commit_message>
<xml_diff>
--- a/SpectraSpectre/MassQL_Queries.xlsx
+++ b/SpectraSpectre/MassQL_Queries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SpectraSpectre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnsondyj\Documents\Projects\DylanJohnson\SpectraSpectre_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174A0E68-98DC-4521-A8F0-76DD3BA5C7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D30AEE-ADEC-4E8C-A42A-9C32F34E1814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7275" yWindow="3870" windowWidth="28980" windowHeight="15300" xr2:uid="{82F246C2-2F34-4170-8964-DC3A51D8D4B5}"/>
+    <workbookView xWindow="2688" yWindow="2292" windowWidth="25920" windowHeight="12144" xr2:uid="{82F246C2-2F34-4170-8964-DC3A51D8D4B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -91,6 +91,36 @@
   </si>
   <si>
     <t>ion_mode</t>
+  </si>
+  <si>
+    <t>threshold</t>
+  </si>
+  <si>
+    <t>not applicable</t>
+  </si>
+  <si>
+    <t>valeryl carnitine-d3</t>
+  </si>
+  <si>
+    <t>C12H20D3NO4</t>
+  </si>
+  <si>
+    <t>octanoyl carnitine-d3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C15H26D3NO4 </t>
+  </si>
+  <si>
+    <t>lauroyl carnitine-d3</t>
+  </si>
+  <si>
+    <t>C19H34D3NO4</t>
+  </si>
+  <si>
+    <t>oleoyl carnitine-d3</t>
+  </si>
+  <si>
+    <t>C25H44D3NO4</t>
   </si>
 </sst>
 </file>
@@ -100,7 +130,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,6 +160,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -151,35 +188,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -188,24 +207,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -550,357 +565,408 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DF47EE8-C1B8-4E0E-AC06-7B0F7F490037}">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" customWidth="1"/>
-    <col min="12" max="13" width="21.42578125" customWidth="1"/>
-    <col min="14" max="14" width="21.85546875" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" customWidth="1"/>
+    <col min="12" max="13" width="21.44140625" customWidth="1"/>
+    <col min="14" max="14" width="21.88671875" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:15" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="O1" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="8">
         <v>206.13458</v>
       </c>
-      <c r="E2">
-        <f t="shared" ref="E2:E3" si="0">D2+1.00725</f>
+      <c r="E2" s="10">
+        <f t="shared" ref="E2:E7" si="0">D2+1.00725</f>
         <v>207.14183</v>
       </c>
-      <c r="F2">
-        <f t="shared" ref="F2:F3" si="1">D2-1.00725</f>
+      <c r="F2" s="10">
+        <f t="shared" ref="F2:F7" si="1">D2-1.00725</f>
         <v>205.12733</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="6">
         <v>1.1299999999999999</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="6">
         <v>1</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="9">
         <v>2.5</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <f>G2-0.1</f>
         <v>1.0299999999999998</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="1">
         <f>G2+0.1</f>
         <v>1.23</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="N2" s="1"/>
+      <c r="O2">
+        <v>0.2</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="8">
         <v>220.15022999999999</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="10">
         <f t="shared" si="0"/>
         <v>221.15747999999999</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="10">
         <f t="shared" si="1"/>
         <v>219.14297999999999</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="6">
         <v>3.35</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="6">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="9">
         <v>2.5</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="1">
         <f t="shared" ref="J3" si="2">G3-0.1</f>
         <v>3.25</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="1">
         <f t="shared" ref="K3" si="3">G3+0.1</f>
         <v>3.45</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="N3" s="1"/>
+      <c r="O3">
+        <v>0.2</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="12"/>
+    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="8">
+        <v>248.18153000000001</v>
+      </c>
+      <c r="E4" s="10">
+        <f t="shared" si="0"/>
+        <v>249.18878000000001</v>
+      </c>
+      <c r="F4" s="10">
+        <f t="shared" si="1"/>
+        <v>247.17428000000001</v>
+      </c>
+      <c r="G4" s="6">
+        <v>4.24</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1</v>
+      </c>
+      <c r="I4" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="J4" s="1">
+        <f>G4-0.1</f>
+        <v>4.1400000000000006</v>
+      </c>
+      <c r="K4" s="1">
+        <f>G4+0.1</f>
+        <v>4.34</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4">
+        <v>0.2</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="7"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="N6" s="4"/>
+    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="8">
+        <v>290.22847999999999</v>
+      </c>
+      <c r="E5" s="10">
+        <f t="shared" si="0"/>
+        <v>291.23572999999999</v>
+      </c>
+      <c r="F5" s="10">
+        <f t="shared" si="1"/>
+        <v>289.22122999999999</v>
+      </c>
+      <c r="G5" s="6">
+        <v>5.83</v>
+      </c>
+      <c r="H5" s="6">
+        <v>1</v>
+      </c>
+      <c r="I5" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" ref="J5:J19" si="4">G5-0.1</f>
+        <v>5.73</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" ref="K5:K19" si="5">G5+0.1</f>
+        <v>5.93</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="6"/>
+      <c r="O5">
+        <v>0.2</v>
+      </c>
     </row>
-    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="8">
+        <v>346.29108000000002</v>
+      </c>
+      <c r="E6" s="10">
+        <f t="shared" si="0"/>
+        <v>347.29833000000002</v>
+      </c>
+      <c r="F6" s="10">
+        <f t="shared" si="1"/>
+        <v>345.28383000000002</v>
+      </c>
+      <c r="G6" s="6">
+        <v>7.49</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="4"/>
+        <v>7.3900000000000006</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="5"/>
+        <v>7.59</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6" s="1"/>
+      <c r="O6">
+        <v>0.2</v>
+      </c>
     </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="8">
+        <v>428.36932999999999</v>
+      </c>
+      <c r="E7" s="10">
+        <f t="shared" si="0"/>
+        <v>429.37657999999999</v>
+      </c>
+      <c r="F7" s="10">
+        <f t="shared" si="1"/>
+        <v>427.36207999999999</v>
+      </c>
+      <c r="G7" s="6">
+        <v>9.17</v>
+      </c>
+      <c r="H7" s="6">
+        <v>1</v>
+      </c>
+      <c r="I7" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="4"/>
+        <v>9.07</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="5"/>
+        <v>9.27</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N7" s="1"/>
+      <c r="O7">
+        <v>0.2</v>
+      </c>
     </row>
-    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="J11" s="3"/>
+    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="N22" s="2"/>
     </row>
-    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="N12" s="3"/>
+    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="N23" s="2"/>
     </row>
-    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="N13" s="3"/>
-    </row>
-    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="N14" s="3"/>
-    </row>
-    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="N15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="N16" s="3"/>
-    </row>
-    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="N17" s="3"/>
-    </row>
-    <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="N18" s="3"/>
-    </row>
-    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="N19" s="3"/>
-    </row>
-    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="N20" s="3"/>
-    </row>
-    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="N21" s="3"/>
-    </row>
-    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="N22" s="3"/>
-    </row>
-    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="N23" s="3"/>
-    </row>
-    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="N24" s="3"/>
+    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="N24" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="E9:E21">
-    <cfRule type="duplicateValues" dxfId="3" priority="12"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5:E6">
-    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
+  <conditionalFormatting sqref="E2:E7">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
removed unused query file columns, calculate mass from monoisotopic using ion mode column, removed integration range
</commit_message>
<xml_diff>
--- a/SpectraSpectre/MassQL_Queries.xlsx
+++ b/SpectraSpectre/MassQL_Queries.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnsondyj\Documents\Projects\DylanJohnson\SpectraSpectre_new\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnsondyj\Documents\Projects\DylanJohnson\SpectraSpectre\SpectraSpectre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D30AEE-ADEC-4E8C-A42A-9C32F34E1814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8870BBA1-6598-44F1-BDF6-792D7E141747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2292" windowWidth="25920" windowHeight="12144" xr2:uid="{82F246C2-2F34-4170-8964-DC3A51D8D4B5}"/>
+    <workbookView xWindow="2688" yWindow="2292" windowWidth="8136" windowHeight="8796" xr2:uid="{82F246C2-2F34-4170-8964-DC3A51D8D4B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -48,18 +48,6 @@
     <t>Monoisotopic</t>
   </si>
   <si>
-    <t>M+H</t>
-  </si>
-  <si>
-    <t>M-H</t>
-  </si>
-  <si>
-    <t>Untargeted F5method7 RT</t>
-  </si>
-  <si>
-    <t>Untargeted F5method7 Comments</t>
-  </si>
-  <si>
     <t>TOLERANCEPPM</t>
   </si>
   <si>
@@ -69,21 +57,12 @@
     <t>RTMAX</t>
   </si>
   <si>
-    <t>INTEGRATION_MIN</t>
-  </si>
-  <si>
-    <t>INTEGRATION_MAX</t>
-  </si>
-  <si>
     <t>acetyl-carnitine-d3</t>
   </si>
   <si>
     <t>C9H14D3NO4</t>
   </si>
   <si>
-    <t>Null</t>
-  </si>
-  <si>
     <t>propionyl carnitine-d3</t>
   </si>
   <si>
@@ -93,9 +72,6 @@
     <t>ion_mode</t>
   </si>
   <si>
-    <t>threshold</t>
-  </si>
-  <si>
     <t>not applicable</t>
   </si>
   <si>
@@ -121,6 +97,9 @@
   </si>
   <si>
     <t>C25H44D3NO4</t>
+  </si>
+  <si>
+    <t>QC_threshold</t>
   </si>
 </sst>
 </file>
@@ -130,7 +109,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,13 +139,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -188,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -213,45 +185,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -262,10 +200,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -565,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DF47EE8-C1B8-4E0E-AC06-7B0F7F490037}">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -577,19 +511,14 @@
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="19.109375" customWidth="1"/>
     <col min="4" max="4" width="18.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" customWidth="1"/>
-    <col min="8" max="8" width="16.88671875" customWidth="1"/>
-    <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" customWidth="1"/>
-    <col min="12" max="13" width="21.44140625" customWidth="1"/>
-    <col min="14" max="14" width="21.88671875" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -602,378 +531,245 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="D2" s="8">
         <v>206.13458</v>
       </c>
-      <c r="E2" s="10">
-        <f t="shared" ref="E2:E7" si="0">D2+1.00725</f>
-        <v>207.14183</v>
-      </c>
-      <c r="F2" s="10">
-        <f t="shared" ref="F2:F7" si="1">D2-1.00725</f>
-        <v>205.12733</v>
-      </c>
-      <c r="G2" s="6">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="H2" s="6">
+      <c r="E2" s="6">
         <v>1</v>
       </c>
-      <c r="I2" s="9">
+      <c r="F2" s="9">
         <v>2.5</v>
       </c>
-      <c r="J2" s="1">
-        <f>G2-0.1</f>
+      <c r="G2" s="1">
         <v>1.0299999999999998</v>
       </c>
-      <c r="K2" s="1">
-        <f>G2+0.1</f>
+      <c r="H2" s="1">
         <v>1.23</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="1"/>
-      <c r="O2">
+      <c r="I2">
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D3" s="8">
         <v>220.15022999999999</v>
       </c>
-      <c r="E3" s="10">
-        <f t="shared" si="0"/>
-        <v>221.15747999999999</v>
-      </c>
-      <c r="F3" s="10">
-        <f t="shared" si="1"/>
-        <v>219.14297999999999</v>
-      </c>
-      <c r="G3" s="6">
-        <v>3.35</v>
-      </c>
-      <c r="H3" s="6">
+      <c r="E3" s="6">
         <v>1</v>
       </c>
-      <c r="I3" s="9">
+      <c r="F3" s="9">
         <v>2.5</v>
       </c>
-      <c r="J3" s="1">
-        <f t="shared" ref="J3" si="2">G3-0.1</f>
+      <c r="G3" s="1">
         <v>3.25</v>
       </c>
-      <c r="K3" s="1">
-        <f t="shared" ref="K3" si="3">G3+0.1</f>
+      <c r="H3" s="1">
         <v>3.45</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="1"/>
-      <c r="O3">
+      <c r="I3">
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D4" s="8">
         <v>248.18153000000001</v>
       </c>
-      <c r="E4" s="10">
-        <f t="shared" si="0"/>
-        <v>249.18878000000001</v>
-      </c>
-      <c r="F4" s="10">
-        <f t="shared" si="1"/>
-        <v>247.17428000000001</v>
-      </c>
-      <c r="G4" s="6">
-        <v>4.24</v>
-      </c>
-      <c r="H4" s="6">
+      <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="I4" s="9">
+      <c r="F4" s="9">
         <v>2.5</v>
       </c>
-      <c r="J4" s="1">
-        <f>G4-0.1</f>
+      <c r="G4" s="1">
         <v>4.1400000000000006</v>
       </c>
-      <c r="K4" s="1">
-        <f>G4+0.1</f>
+      <c r="H4" s="1">
         <v>4.34</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="I4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N4" s="1"/>
-      <c r="O4">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="B5" s="9" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D5" s="8">
         <v>290.22847999999999</v>
       </c>
-      <c r="E5" s="10">
-        <f t="shared" si="0"/>
-        <v>291.23572999999999</v>
-      </c>
-      <c r="F5" s="10">
-        <f t="shared" si="1"/>
-        <v>289.22122999999999</v>
-      </c>
-      <c r="G5" s="6">
-        <v>5.83</v>
-      </c>
-      <c r="H5" s="6">
+      <c r="E5" s="6">
         <v>1</v>
       </c>
-      <c r="I5" s="9">
+      <c r="F5" s="9">
         <v>2.5</v>
       </c>
-      <c r="J5" s="1">
-        <f t="shared" ref="J5:J19" si="4">G5-0.1</f>
+      <c r="G5" s="1">
         <v>5.73</v>
       </c>
-      <c r="K5" s="1">
-        <f t="shared" ref="K5:K19" si="5">G5+0.1</f>
+      <c r="H5" s="1">
         <v>5.93</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N5" s="6"/>
-      <c r="O5">
+      <c r="I5">
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D6" s="8">
         <v>346.29108000000002</v>
       </c>
-      <c r="E6" s="10">
-        <f t="shared" si="0"/>
-        <v>347.29833000000002</v>
-      </c>
-      <c r="F6" s="10">
-        <f t="shared" si="1"/>
-        <v>345.28383000000002</v>
-      </c>
-      <c r="G6" s="6">
-        <v>7.49</v>
-      </c>
-      <c r="H6" s="6">
+      <c r="E6" s="6">
         <v>1</v>
       </c>
-      <c r="I6" s="9">
+      <c r="F6" s="9">
         <v>2.5</v>
       </c>
-      <c r="J6" s="1">
-        <f t="shared" si="4"/>
+      <c r="G6" s="1">
         <v>7.3900000000000006</v>
       </c>
-      <c r="K6" s="1">
-        <f t="shared" si="5"/>
+      <c r="H6" s="1">
         <v>7.59</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N6" s="1"/>
-      <c r="O6">
+      <c r="I6">
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="D7" s="8">
         <v>428.36932999999999</v>
       </c>
-      <c r="E7" s="10">
-        <f t="shared" si="0"/>
-        <v>429.37657999999999</v>
-      </c>
-      <c r="F7" s="10">
-        <f t="shared" si="1"/>
-        <v>427.36207999999999</v>
-      </c>
-      <c r="G7" s="6">
-        <v>9.17</v>
-      </c>
-      <c r="H7" s="6">
+      <c r="E7" s="6">
         <v>1</v>
       </c>
-      <c r="I7" s="9">
+      <c r="F7" s="9">
         <v>2.5</v>
       </c>
-      <c r="J7" s="1">
-        <f t="shared" si="4"/>
+      <c r="G7" s="1">
         <v>9.07</v>
       </c>
-      <c r="K7" s="1">
-        <f t="shared" si="5"/>
+      <c r="H7" s="1">
         <v>9.27</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N7" s="1"/>
-      <c r="O7">
+      <c r="I7">
         <v>0.2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="N24" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="E2:E7">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="905c205a-84eb-47d2-bf11-395d8bb54267">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="13fdb75f-0e59-4cb7-b51e-6482710d85d6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AEA5DB7D0DA16943820F736AA1F61F70" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ecd8950973e592508b631a6fa13ac323">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="905c205a-84eb-47d2-bf11-395d8bb54267" xmlns:ns3="13fdb75f-0e59-4cb7-b51e-6482710d85d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fe1da0bb70e6922348720235f7dbbf5d" ns2:_="" ns3:_="">
     <xsd:import namespace="905c205a-84eb-47d2-bf11-395d8bb54267"/>
@@ -1178,27 +974,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="905c205a-84eb-47d2-bf11-395d8bb54267">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="13fdb75f-0e59-4cb7-b51e-6482710d85d6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6559989F-897C-48F4-A6D0-3A8AD2599F97}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="905c205a-84eb-47d2-bf11-395d8bb54267"/>
+    <ds:schemaRef ds:uri="13fdb75f-0e59-4cb7-b51e-6482710d85d6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF9ACDF3-3968-4F27-AF9B-C0DA3431C13D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86646020-003E-4A6E-B444-74F61888A5E7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1215,23 +1010,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6559989F-897C-48F4-A6D0-3A8AD2599F97}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="905c205a-84eb-47d2-bf11-395d8bb54267"/>
-    <ds:schemaRef ds:uri="13fdb75f-0e59-4cb7-b51e-6482710d85d6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF9ACDF3-3968-4F27-AF9B-C0DA3431C13D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MS2 queries now select only most intense scan. Query results are now split by collision method and energy if applicable. MS2 scan images are exported to output directory.
</commit_message>
<xml_diff>
--- a/SpectraSpectre/MassQL_Queries.xlsx
+++ b/SpectraSpectre/MassQL_Queries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnsondyj\Documents\Projects\DylanJohnson\SpectraSpectre\SpectraSpectre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnsondyj\Documents\Projects\DylanJohnson\SpectraSpectre_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8870BBA1-6598-44F1-BDF6-792D7E141747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC5AECF-DA35-4446-B413-B9E9889E137D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2292" windowWidth="8136" windowHeight="8796" xr2:uid="{82F246C2-2F34-4170-8964-DC3A51D8D4B5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{82F246C2-2F34-4170-8964-DC3A51D8D4B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>QC_threshold</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -499,26 +505,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DF47EE8-C1B8-4E0E-AC06-7B0F7F490037}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.453125" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" customWidth="1"/>
+    <col min="3" max="3" width="21.453125" customWidth="1"/>
+    <col min="4" max="4" width="19.08984375" customWidth="1"/>
+    <col min="5" max="5" width="18.453125" customWidth="1"/>
+    <col min="6" max="6" width="16.90625" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="14.36328125" customWidth="1"/>
+    <col min="9" max="9" width="15.54296875" customWidth="1"/>
+    <col min="10" max="10" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -526,28 +533,31 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -555,28 +565,31 @@
         <v>12</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="8">
+      <c r="E2" s="8">
         <v>206.13458</v>
       </c>
-      <c r="E2" s="6">
+      <c r="F2" s="6">
         <v>1</v>
       </c>
-      <c r="F2" s="9">
+      <c r="G2" s="9">
         <v>2.5</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>1.0299999999999998</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>1.23</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
@@ -584,28 +597,31 @@
         <v>12</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="8">
+      <c r="E3" s="8">
         <v>220.15022999999999</v>
       </c>
-      <c r="E3" s="6">
+      <c r="F3" s="6">
         <v>1</v>
       </c>
-      <c r="F3" s="9">
+      <c r="G3" s="9">
         <v>2.5</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>3.25</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>3.45</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
@@ -613,28 +629,31 @@
         <v>12</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="8">
+      <c r="E4" s="8">
         <v>248.18153000000001</v>
       </c>
-      <c r="E4" s="6">
+      <c r="F4" s="6">
         <v>1</v>
       </c>
-      <c r="F4" s="9">
+      <c r="G4" s="9">
         <v>2.5</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>4.1400000000000006</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>4.34</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
@@ -642,28 +661,31 @@
         <v>12</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="8">
+      <c r="E5" s="8">
         <v>290.22847999999999</v>
       </c>
-      <c r="E5" s="6">
+      <c r="F5" s="6">
         <v>1</v>
       </c>
-      <c r="F5" s="9">
+      <c r="G5" s="9">
         <v>2.5</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>5.73</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>5.93</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>17</v>
       </c>
@@ -671,28 +693,31 @@
         <v>12</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="8">
+      <c r="E6" s="8">
         <v>346.29108000000002</v>
       </c>
-      <c r="E6" s="6">
+      <c r="F6" s="6">
         <v>1</v>
       </c>
-      <c r="F6" s="9">
+      <c r="G6" s="9">
         <v>2.5</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>7.3900000000000006</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>7.59</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
@@ -700,47 +725,53 @@
         <v>12</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="8">
+      <c r="E7" s="8">
         <v>428.36932999999999</v>
       </c>
-      <c r="E7" s="6">
+      <c r="F7" s="6">
         <v>1</v>
       </c>
-      <c r="F7" s="9">
+      <c r="G7" s="9">
         <v>2.5</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>9.07</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>9.27</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>0.2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -750,26 +781,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="905c205a-84eb-47d2-bf11-395d8bb54267">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="13fdb75f-0e59-4cb7-b51e-6482710d85d6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AEA5DB7D0DA16943820F736AA1F61F70" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ecd8950973e592508b631a6fa13ac323">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="905c205a-84eb-47d2-bf11-395d8bb54267" xmlns:ns3="13fdb75f-0e59-4cb7-b51e-6482710d85d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fe1da0bb70e6922348720235f7dbbf5d" ns2:_="" ns3:_="">
     <xsd:import namespace="905c205a-84eb-47d2-bf11-395d8bb54267"/>
@@ -974,26 +985,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6559989F-897C-48F4-A6D0-3A8AD2599F97}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="905c205a-84eb-47d2-bf11-395d8bb54267"/>
-    <ds:schemaRef ds:uri="13fdb75f-0e59-4cb7-b51e-6482710d85d6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="905c205a-84eb-47d2-bf11-395d8bb54267">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="13fdb75f-0e59-4cb7-b51e-6482710d85d6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF9ACDF3-3968-4F27-AF9B-C0DA3431C13D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86646020-003E-4A6E-B444-74F61888A5E7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1010,4 +1022,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6559989F-897C-48F4-A6D0-3A8AD2599F97}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="905c205a-84eb-47d2-bf11-395d8bb54267"/>
+    <ds:schemaRef ds:uri="13fdb75f-0e59-4cb7-b51e-6482710d85d6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF9ACDF3-3968-4F27-AF9B-C0DA3431C13D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>